<commit_message>
Nuevas actualizaciones en hubs-equipos
</commit_message>
<xml_diff>
--- a/EquipoGeko/ProyectoDojoGeko/ProyectoDojoGeko/wwwroot/plantillas/PlantillaCargaMasivaSolicitudes.xlsx
+++ b/EquipoGeko/ProyectoDojoGeko/ProyectoDojoGeko/wwwroot/plantillas/PlantillaCargaMasivaSolicitudes.xlsx
@@ -5,24 +5,25 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/823064aeb5a082ef/Documentos/Escritorio/ProyectoGrupalGekoMayo/DojoNet/EquipoGeko/ProyectoDojoGeko/ProyectoDojoGeko/wwwroot/plantillas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC3488A-EDE7-4B97-9167-A7EC7B7DE5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9CC3488A-EDE7-4B97-9167-A7EC7B7DE5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7D85DA7-4500-4F44-8B7A-A7A96FC2E67E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instrucciones" sheetId="1" r:id="rId1"/>
-    <sheet name="SolicitudEncabezado" sheetId="2" r:id="rId2"/>
-    <sheet name="SolicitudDetalle" sheetId="3" r:id="rId3"/>
+    <sheet name="Empleado" sheetId="4" r:id="rId2"/>
+    <sheet name="SolicitudEncabezado" sheetId="2" r:id="rId3"/>
+    <sheet name="SolicitudDetalle" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="77">
   <si>
     <t># Plantilla de Carga Masiva de Solicitudes</t>
   </si>
@@ -90,12 +91,6 @@
     <t>- Las solicitudes se crearán con estado 'Pendiente' por defecto</t>
   </si>
   <si>
-    <t>## Soporte</t>
-  </si>
-  <si>
-    <t>Para cualquier duda o problema con la plantilla, contacte al equipo de desarrollo del proyecto Dojo Geko.</t>
-  </si>
-  <si>
     <t>IdSolicitud</t>
   </si>
   <si>
@@ -160,13 +155,112 @@
   </si>
   <si>
     <t>09/09/2025</t>
+  </si>
+  <si>
+    <t>TipoDocumento</t>
+  </si>
+  <si>
+    <t>DPI</t>
+  </si>
+  <si>
+    <t>Pasaporte</t>
+  </si>
+  <si>
+    <t>NombresEmpleado</t>
+  </si>
+  <si>
+    <t>ApellidosEmpleado</t>
+  </si>
+  <si>
+    <t>FechaNacimiento</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>CorreoPersonal</t>
+  </si>
+  <si>
+    <t>CorreoInstitucional</t>
+  </si>
+  <si>
+    <t>País</t>
+  </si>
+  <si>
+    <t>Teléfono</t>
+  </si>
+  <si>
+    <t>FechaIngreso</t>
+  </si>
+  <si>
+    <t>TipoContrato</t>
+  </si>
+  <si>
+    <t>Puesto</t>
+  </si>
+  <si>
+    <t>DiasVacacionesAcumulados</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Pérez</t>
+  </si>
+  <si>
+    <t>Ciudad de Guatemala</t>
+  </si>
+  <si>
+    <t>Planilla</t>
+  </si>
+  <si>
+    <t>Desarrollador</t>
+  </si>
+  <si>
+    <t>A12345678901234</t>
+  </si>
+  <si>
+    <t>México</t>
+  </si>
+  <si>
+    <t>Ana</t>
+  </si>
+  <si>
+    <t>López</t>
+  </si>
+  <si>
+    <t>Ciudad de México</t>
+  </si>
+  <si>
+    <t>Facturado</t>
+  </si>
+  <si>
+    <t>Analista</t>
+  </si>
+  <si>
+    <t>Ejemplos</t>
+  </si>
+  <si>
+    <t>juan@gmail.com</t>
+  </si>
+  <si>
+    <t>ana@gmail.com</t>
+  </si>
+  <si>
+    <t>juan@digitalgeko.com</t>
+  </si>
+  <si>
+    <t>ana@digitalgeko.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +272,44 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -197,16 +329,49 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -507,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A30"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,26 +790,220 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DA28FF-8055-4CA9-B5A7-FF68B579DD99}">
+  <dimension ref="A1:V6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="9" width="34.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" customWidth="1"/>
+    <col min="13" max="13" width="27.140625" customWidth="1"/>
+    <col min="14" max="14" width="23.140625" customWidth="1"/>
+    <col min="15" max="15" width="19.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="3">
+        <v>5871115680101</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="4">
+        <v>32874</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L2" s="3">
+        <v>55551234</v>
+      </c>
+      <c r="M2" s="4">
+        <v>45413</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+    </row>
+    <row r="3" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="4">
+        <v>31121</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="3">
+        <v>55559876</v>
+      </c>
+      <c r="M3" s="4">
+        <v>45392</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P3" s="3">
+        <v>5</v>
+      </c>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H6" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="R2:V3"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{14F7C2C6-C2BF-413C-B4F0-F8C7835428D8}"/>
+    <hyperlink ref="K2" r:id="rId2" xr:uid="{5CA88E92-C789-46EA-B173-D5884706763F}"/>
+    <hyperlink ref="J3" r:id="rId3" xr:uid="{86ADFFAD-B55A-4F3C-90E8-B37A2B0F74EF}"/>
+    <hyperlink ref="K3" r:id="rId4" xr:uid="{175241D6-2EDA-4442-97DA-C9EB29FC44CC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W44" sqref="W44"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -663,37 +1022,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -704,19 +1063,19 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>5</v>
       </c>
       <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
         <v>36</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -725,7 +1084,7 @@
         <v>201</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -733,7 +1092,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -750,19 +1109,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -773,10 +1132,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>5</v>

</xml_diff>